<commit_message>
add hyperlinks to CVs in templates
</commit_message>
<xml_diff>
--- a/CUAHSI_documentation/Advanced_Formatting_Template.xlsx
+++ b/CUAHSI_documentation/Advanced_Formatting_Template.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="261">
   <si>
     <t>Field Name</t>
   </si>
@@ -789,9 +789,6 @@
     <t>Link to additional metadata reference material.</t>
   </si>
   <si>
-    <t>Controlled vocabulary specificying the sample type. This should be from the SampleType controlled vocabulary.</t>
-  </si>
-  <si>
     <t>Code or label used to identify and track lab sample or sample container (e.g. bottoe) during lab analysis.</t>
   </si>
   <si>
@@ -856,9 +853,6 @@
   </si>
   <si>
     <t>OffsetUnitsName</t>
-  </si>
-  <si>
-    <t>Full name of units of the Offset Value. This should be from the Units controlled vocabulary.</t>
   </si>
   <si>
     <t>Full text description of the offset type.</t>
@@ -1118,12 +1112,27 @@
   <si>
     <t>We recommend only using this template to augment the standard template with Qualifiers and/or Categories.</t>
   </si>
+  <si>
+    <t>Controlled vocabulary specificying the sample type. This should be from the SampleType controlled vocabulary: http://his.cuahsi.org/mastercvreg/edit_cv11.aspx?tbl=SampleTypeCV</t>
+  </si>
+  <si>
+    <t>Mandatory if table is used; Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>Mandatory; Foreign Key; Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>Full name of units of the Offset Value. This should be from the Units controlled vocabulary: http://his.cuahsi.org/mastercvreg/edit_cv11.aspx?tbl=Units</t>
+  </si>
+  <si>
+    <t>Mandatory if table is used; Foreign Key; Controlled Vocabulary</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1301,6 +1310,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1710,7 +1727,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1753,8 +1770,9 @@
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1795,6 +1813,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1828,8 +1847,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1849,21 +1880,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1897,6 +1919,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2221,34 +2244,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B5" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -2267,17 +2290,17 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
-        <v>256</v>
+      <c r="B11" s="22" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="s">
-        <v>257</v>
+      <c r="B12" s="22" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -2300,18 +2323,18 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
@@ -2343,19 +2366,19 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="32"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2366,57 +2389,57 @@
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
+      <c r="B23" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="7"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
+      <c r="B26" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2492,7 +2515,7 @@
         <v>23</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>25</v>
@@ -2501,13 +2524,13 @@
         <v>48</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>27</v>
@@ -2577,7 +2600,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -2586,13 +2609,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
@@ -2604,10 +2627,10 @@
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>254</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
+        <v>252</v>
+      </c>
+      <c r="L3" s="45" t="s">
+        <v>258</v>
       </c>
       <c r="M3" t="s">
         <v>24</v>
@@ -2633,55 +2656,55 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="J4" s="14" t="s">
+      <c r="K4" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="R4" s="16" t="s">
         <v>181</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -2692,13 +2715,13 @@
         <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H5" t="s">
         <v>105</v>
@@ -2720,8 +2743,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2786,13 +2812,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>184</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2858,10 +2884,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>186</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2931,10 +2957,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3001,10 +3027,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>190</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3042,10 +3068,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>47</v>
@@ -3065,32 +3091,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>127</v>
+      <c r="C3" s="46" t="s">
+        <v>260</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>193</v>
+        <v>259</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3108,6 +3134,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3163,10 +3192,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3189,9 +3218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:P13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3199,572 +3226,574 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="36"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="39"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-    </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B24:P25"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B12:P13"/>
+    <mergeCell ref="B14:P15"/>
+    <mergeCell ref="B16:P17"/>
+    <mergeCell ref="B18:P19"/>
+    <mergeCell ref="B22:P23"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B26:P27"/>
     <mergeCell ref="B28:P29"/>
@@ -3781,13 +3810,11 @@
     <mergeCell ref="B6:P7"/>
     <mergeCell ref="B8:P9"/>
     <mergeCell ref="B10:P11"/>
-    <mergeCell ref="B24:P25"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B12:P13"/>
-    <mergeCell ref="B14:P15"/>
-    <mergeCell ref="B16:P17"/>
-    <mergeCell ref="B18:P19"/>
-    <mergeCell ref="B22:P23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3902,19 +3929,19 @@
       <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="45" t="s">
         <v>97</v>
       </c>
       <c r="H3" t="s">
@@ -3923,13 +3950,13 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="45" t="s">
         <v>97</v>
       </c>
       <c r="M3" t="s">
@@ -3941,40 +3968,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="E4" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="F4" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="I4" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="J4" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="K4" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="M4" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -4019,6 +4046,16 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="K3" r:id="rId5"/>
+    <hyperlink ref="J3" r:id="rId6"/>
+    <hyperlink ref="L3" r:id="rId7"/>
+    <hyperlink ref="G3" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4042,7 +4079,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>45</v>
@@ -4084,7 +4121,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>145</v>
@@ -4254,14 +4291,14 @@
       <c r="E3" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>230</v>
+      <c r="F3" s="45" t="s">
+        <v>228</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>232</v>
+      <c r="H3" s="45" t="s">
+        <v>230</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -4269,8 +4306,8 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>232</v>
+      <c r="K3" s="45" t="s">
+        <v>230</v>
       </c>
       <c r="L3" t="s">
         <v>14</v>
@@ -4284,7 +4321,7 @@
       <c r="O3" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="45" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4293,7 +4330,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>148</v>
@@ -4305,13 +4342,13 @@
         <v>150</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>151</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>152</v>
@@ -4320,7 +4357,7 @@
         <v>153</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>154</v>
@@ -4335,7 +4372,7 @@
         <v>157</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4368,6 +4405,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="P3" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4399,7 +4442,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>64</v>
@@ -4546,7 +4589,7 @@
       <c r="M3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="45" t="s">
         <v>97</v>
       </c>
       <c r="O3" t="s">
@@ -4567,7 +4610,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>158</v>
@@ -4576,7 +4619,7 @@
         <v>159</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>160</v>
@@ -4600,10 +4643,10 @@
         <v>166</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O4" s="14" t="s">
         <v>167</v>
@@ -4612,7 +4655,7 @@
         <v>168</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R4" s="14" t="s">
         <v>169</v>
@@ -4669,8 +4712,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4720,28 +4766,28 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>127</v>
+      <c r="B3" s="45" t="s">
+        <v>257</v>
       </c>
       <c r="C3" t="s">
         <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>171</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4759,6 +4805,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="Mandatory if table is used; Foreign Key"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4828,7 +4877,7 @@
         <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
         <v>126</v>
@@ -4842,19 +4891,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>175</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4928,7 +4977,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -4942,13 +4991,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" t="s">
         <v>177</v>
-      </c>
-      <c r="C4" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4956,13 +5005,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>